<commit_message>
gamelogic almost fully implemented
</commit_message>
<xml_diff>
--- a/gameDesign/techs_amelios.xlsx
+++ b/gameDesign/techs_amelios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cours\Mobile_Dev\Android\proj\PaintClicker\gameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F686F820-4639-4991-9925-1442B139CB9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE3DD29E-8865-44E1-BE57-81A6BB44BAEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20685" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="techs" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +613,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,6 +709,19 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="D4">
+        <v>200</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <f>D4*E4^F4</f>
+        <v>5400</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>33</v>
       </c>

</xml_diff>